<commit_message>
Correlation bar chart saved
</commit_message>
<xml_diff>
--- a/auxillary_files/bar_chart_feature_correlation_with_arr_delay.xlsx
+++ b/auxillary_files/bar_chart_feature_correlation_with_arr_delay.xlsx
@@ -1,39 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christiantruchsess/Documents/Professional/Programming/Lighthouse Labs/data_bootcamp/Mid_Term_Project/Predicting_Flight_Delays/auxillary_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Predicting_Flight_Delays\auxillary_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C486192-9222-3646-9E22-CFC6973DA956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51393CC4-F921-42E4-8420-DB1C472B181C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{2E02159A-2CBF-E64B-BB9C-2CDE8874EF67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E02159A-2CBF-E64B-BB9C-2CDE8874EF67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$3:$B$55</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$C$55</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3:$B$55</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3:$C$55</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -247,7 +232,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,7 +250,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -682,7 +667,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -720,7 +705,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1571804496"/>
@@ -752,6 +737,32 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
+                  <a:t>Features Correlation with Target</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU" sz="2400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -777,7 +788,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -809,7 +820,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1571787872"/>
@@ -824,37 +835,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -888,7 +868,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1447,15 +1427,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>110490</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>41564</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>96981</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1484,9 +1464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1524,7 +1504,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1630,7 +1610,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1782,14 +1762,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93168B-400E-D348-AF84-232B6FB9F70F}">
   <dimension ref="B2:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="33" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added images for presentation
</commit_message>
<xml_diff>
--- a/auxillary_files/bar_chart_feature_correlation_with_arr_delay.xlsx
+++ b/auxillary_files/bar_chart_feature_correlation_with_arr_delay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Predicting_Flight_Delays\auxillary_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christiantruchsess/Documents/Professional/Programming/Lighthouse Labs/data_bootcamp/Mid_Term_Project/Predicting_Flight_Delays/auxillary_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51393CC4-F921-42E4-8420-DB1C472B181C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07E7BAF-F5FF-4049-A0EB-3645004D607C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E02159A-2CBF-E64B-BB9C-2CDE8874EF67}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{2E02159A-2CBF-E64B-BB9C-2CDE8874EF67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -250,7 +250,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -263,7 +263,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2600698845203559"/>
+          <c:y val="9.5556063270206687E-2"/>
+          <c:w val="0.71992572575837566"/>
+          <c:h val="0.8957135353617276"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -642,6 +652,40 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Features</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.303293370939106E-2"/>
+              <c:y val="0.49785704519965562"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -667,7 +711,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -693,7 +737,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -705,7 +749,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1571804496"/>
@@ -763,6 +807,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.30847045974142834"/>
+              <c:y val="1.8173403029440441E-2"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -788,7 +840,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -820,7 +872,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1571787872"/>
@@ -868,7 +920,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1426,16 +1478,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>110490</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>41564</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>96981</xdr:rowOff>
+      <xdr:colOff>247304</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>157941</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1464,9 +1516,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1504,7 +1556,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1610,7 +1662,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1762,14 +1814,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93168B-400E-D348-AF84-232B6FB9F70F}">
   <dimension ref="B2:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="32.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>